<commit_message>
Update 2p3. Added templates for formula student suspension, torque vectoring, four-wheel steering
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Body/Sedan/sm_car_data_BodyGeometry_Sedan.xlsx
+++ b/Libraries/Vehicle/Body/Sedan/sm_car_data_BodyGeometry_Sedan.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Vehicle\Body\Sedan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DA7F7F-1D67-4E35-8816-63467FE64D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE36AD-1C8D-4DEF-B25F-B8313E0FBDED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11430" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11430" activeTab="1" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sedan_HambaLG" sheetId="1" r:id="rId1"/>
+    <sheet name="FSAE_Achilles" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>Units</t>
   </si>
@@ -90,6 +91,9 @@
   </si>
   <si>
     <t>Sedan_HambaLG</t>
+  </si>
+  <si>
+    <t>FSAE_Achilles</t>
   </si>
 </sst>
 </file>
@@ -514,6 +518,209 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E9" sqref="E9"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="10" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0.32250000000000001</v>
+      </c>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="13"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="L9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+      <c r="H10" s="16">
+        <v>1</v>
+      </c>
+      <c r="L10" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6247D35C-52BF-43DD-A916-4B6ACA453410}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:L10"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
@@ -578,7 +785,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -628,7 +835,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L6" s="13"/>
     </row>

</xml_diff>